<commit_message>
feat: add unduh file pdf
</commit_message>
<xml_diff>
--- a/data_siswa.xlsx
+++ b/data_siswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\App-Development\ceklulus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FF1F1A-0F79-4C31-BDBF-5D5B3ED8C957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E77252-E842-4E32-A181-39C64BCEFD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{12D39D77-401A-4D23-BD2A-539CB254051B}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>status_kelulusan</t>
   </si>
   <si>
-    <t>pesan</t>
-  </si>
-  <si>
     <t>Jhon Dee</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>TIDAK LULUS</t>
+  </si>
+  <si>
+    <t>file_pdf</t>
   </si>
 </sst>
 </file>
@@ -95,13 +95,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -111,9 +108,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,17 +426,17 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="90.42578125" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -458,44 +452,44 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>12345</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="4">
+        <v>39764</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>A2&amp;".pdf"</f>
+        <v>12345.pdf</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>12345</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>12346</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5">
-        <v>39764</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C3" s="4">
+        <v>39398</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="str">
-        <f>IF(D2="lulus", "Selamat! Anda dinyatakan LULUS sebagai siswa MA Nurul Ummah. Semoga prestasi ini menjadi awal dari kesuksesan Anda di masa depan. Silakan mengikuti proses pengambilan ijazah pada tanggal 10-15 Mei 2025.", "Mohon maaf, Anda dinyatakan TIDAK LULUS tahun ajaran ini. Jangan berkecil hati, ini bukan akhir dari perjalanan pendidikan Anda. Silakan menghubungi Bapak/Ibu wali kelas untuk konsultasi pada tanggal 5 Mei 2025.")</f>
-        <v>Selamat! Anda dinyatakan LULUS sebagai siswa MA Nurul Ummah. Semoga prestasi ini menjadi awal dari kesuksesan Anda di masa depan. Silakan mengikuti proses pengambilan ijazah pada tanggal 10-15 Mei 2025.</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>12346</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5">
-        <v>39398</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="6" t="str">
-        <f>IF(D3="lulus", "Selamat! Anda dinyatakan LULUS sebagai siswa MA Nurul Ummah. Semoga prestasi ini menjadi awal dari kesuksesan Anda di masa depan. Silakan mengikuti proses pengambilan ijazah pada tanggal 10-15 Mei 2025.", "Mohon maaf, Anda dinyatakan TIDAK LULUS tahun ajaran ini. Jangan berkecil hati, ini bukan akhir dari perjalanan pendidikan Anda. Silakan menghubungi Bapak/Ibu wali kelas untuk konsultasi pada tanggal 5 Mei 2025.")</f>
-        <v>Mohon maaf, Anda dinyatakan TIDAK LULUS tahun ajaran ini. Jangan berkecil hati, ini bukan akhir dari perjalanan pendidikan Anda. Silakan menghubungi Bapak/Ibu wali kelas untuk konsultasi pada tanggal 5 Mei 2025.</v>
+      <c r="E3" s="2" t="str">
+        <f>A3&amp;".pdf"</f>
+        <v>12346.pdf</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add schedule to access kelulusan form
</commit_message>
<xml_diff>
--- a/data_siswa.xlsx
+++ b/data_siswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\App-Development\ceklulus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E77252-E842-4E32-A181-39C64BCEFD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912CA5A0-B417-430F-9732-7DE3E89292CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{12D39D77-401A-4D23-BD2A-539CB254051B}"/>
   </bookViews>
@@ -425,13 +425,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC97B2A-D0EC-49CF-A1F8-0D61CBB6B1E8}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" bestFit="1" customWidth="1"/>

</xml_diff>